<commit_message>
Saved Gaps Excel sheet
</commit_message>
<xml_diff>
--- a/FibPrimeGaps.xlsx
+++ b/FibPrimeGaps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/siddhantdoshi/Documents/Competitions/ST Yau Research Paper/2020/Math/ST-Yau-Math-031/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78147C72-9B7F-7444-94C6-F401E3EA19F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5101C40B-0A08-D846-B76E-3A58A7EABD79}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A65D2994-66A2-5346-839E-C7A732D7265C}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Fib Prime Differences</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>ln(gaps)</t>
-  </si>
-  <si>
-    <t>3571035606419098607209077741390634544455699265828433067940419974763010711027675704833435635185100078003041954440805185626309000273864989339446192101928567683526834688317544232342179785257659210407472913166815765568614907731352148617828777165608796863682661173653518849263937754319251168963223411300758802871692449806988379419312475160101016317043499635834003619108099258477213008027417055194123065229</t>
   </si>
 </sst>
 </file>
@@ -411,7 +408,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -716,19 +713,7 @@
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="e">
-        <f t="shared" si="0"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="D21">
-        <v>2.0747194439999999</v>
-      </c>
+      <c r="B21" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>